<commit_message>
Finished testing player class.
Added 4 tests for the game class.
</commit_message>
<xml_diff>
--- a/TDS.xlsx
+++ b/TDS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Djole\IdeaProjects\qa-job-fair-puzzle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79F9BC5-4153-4BA1-8CC6-F602A11D6CBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B7FEF1-D7B9-4C35-A464-88374FC51EA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17475" yWindow="480" windowWidth="16140" windowHeight="11595" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
   <si>
     <t>Description</t>
   </si>
@@ -154,12 +154,6 @@
     </r>
   </si>
   <si>
-    <t>Upon instantiation player's HP is able to be set to more than 20. Documentation states that starting HP should always be 20.</t>
-  </si>
-  <si>
-    <t>Upon instantiation player's HP is able to be set to less than 20. Documentation states that starting HP should always be 20.</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Total amount of player HP at the start of the game (expected -&gt; </t>
     </r>
@@ -285,6 +279,33 @@
       <t>)</t>
     </r>
   </si>
+  <si>
+    <t>Verify total amount of player HP cannot be set to a negative value</t>
+  </si>
+  <si>
+    <t>Upon instantiation player's HP is able to be set to less than 20. Documentation states that starting HP should always be 20.  -make hp a constant value of 20</t>
+  </si>
+  <si>
+    <t>Upon instantiation player's HP is able to be set to more than 20. Documentation states that starting HP should always be 20.  -make hp a constant value of 20</t>
+  </si>
+  <si>
+    <t>Upon instantiation player's HP is able to be set to a negative value. -make hp a constant value of 20</t>
+  </si>
+  <si>
+    <t>Game doesn't end when one player takes 20 damage, which goes back to Player class testing. See test #3.</t>
+  </si>
+  <si>
+    <t>A player is able to play multiple cards in a single turn.</t>
+  </si>
+  <si>
+    <t>Verify you cannot draw after playing a turn</t>
+  </si>
+  <si>
+    <t>Player can both play and draw in the same turn</t>
+  </si>
+  <si>
+    <t>Test whether the game actually starts</t>
+  </si>
 </sst>
 </file>
 
@@ -401,7 +422,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -444,6 +465,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -831,7 +859,7 @@
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -915,7 +943,7 @@
     </row>
     <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>8</v>
@@ -941,7 +969,7 @@
     </row>
     <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>8</v>
@@ -953,7 +981,7 @@
     </row>
     <row r="9" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>6</v>
@@ -1000,7 +1028,7 @@
     </row>
     <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>8</v>
@@ -1010,36 +1038,44 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C16" s="15"/>
+    <row r="16" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>31</v>
+      </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -1052,30 +1088,66 @@
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>32</v>
+      </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B20" s="7"/>
+      <c r="A20" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>35</v>
+      </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B21" s="7"/>
+    <row r="21" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>33</v>
+      </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B22" s="7"/>
+      <c r="A22" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="18"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
@@ -1105,27 +1177,18 @@
       <c r="F26" s="4"/>
     </row>
     <row r="27" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A27" s="9" t="s">
-        <v>9</v>
-      </c>
       <c r="B27" s="7"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>10</v>
-      </c>
       <c r="B28" s="7"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>11</v>
-      </c>
       <c r="B29" s="7"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -1138,15 +1201,15 @@
       <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A31" s="9" t="s">
+        <v>12</v>
+      </c>
       <c r="B31" s="7"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A32" s="9" t="s">
-        <v>12</v>
-      </c>
       <c r="B32" s="7"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -6114,15 +6177,15 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="B20:B147 B3:B6 B8:B11 B13:B15 B17" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="B3:B6 B8:B11 B13:B15 B17 B21:B147" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Passed,In Progress,Failed"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup scale="64" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup scale="54" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <colBreaks count="1" manualBreakCount="1">
-    <brk id="4" max="1048575" man="1"/>
+    <brk id="6" max="1048575" man="1"/>
   </colBreaks>
 </worksheet>
 </file>
</xml_diff>